<commit_message>
Completed Lesson 16 JMeter
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoNguyen\OneDrive\Máy tính\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncbao\Downloads\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46310B5F-34AE-4E39-94FD-0448049706BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="COOLMATE-004" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>No.</t>
   </si>
@@ -60,20 +59,53 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>Added products in cart match with the selected ones</t>
+  </si>
+  <si>
     <t>TS001-Add Product To Cart</t>
   </si>
   <si>
     <t xml:space="preserve">TC001-Add product to cart the product page </t>
   </si>
   <si>
-    <t xml:space="preserve">TC001-Add product to cart the product detail page </t>
+    <t>Add a product from the product page and verify the added product in cart</t>
+  </si>
+  <si>
+    <t>The added product in cart match with the selected one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC002-Add product to cart the product detail page </t>
+  </si>
+  <si>
+    <t>The number of products that have been added is updated in cart</t>
+  </si>
+  <si>
+    <t>Added product in cart match with the selected options</t>
+  </si>
+  <si>
+    <t>Add a product with many color and size pairs from the product page and verify added product in cart</t>
+  </si>
+  <si>
+    <t>Add a product with many color and size pairs from the product detail page and verify added product in cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC003-Add product to cart from product page with many options </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC004-Add product to cart from product detail page with many options </t>
+  </si>
+  <si>
+    <t>Add products from the product page to cart and verify added products in cart</t>
+  </si>
+  <si>
+    <t>Go to the product detail page to add product to cart of the same color  and size that was previously added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,36 +114,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="13"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,34 +138,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -157,16 +165,29 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -177,48 +198,105 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="2" builtinId="20"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,92 +574,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="69" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed Lesson 17 JMeter
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>No.</t>
   </si>
@@ -68,18 +68,9 @@
     <t xml:space="preserve">TC001-Add product to cart the product page </t>
   </si>
   <si>
-    <t>Add a product from the product page and verify the added product in cart</t>
-  </si>
-  <si>
-    <t>The added product in cart match with the selected one</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC002-Add product to cart the product detail page </t>
   </si>
   <si>
-    <t>The number of products that have been added is updated in cart</t>
-  </si>
-  <si>
     <t>Added product in cart match with the selected options</t>
   </si>
   <si>
@@ -98,7 +89,19 @@
     <t>Add products from the product page to cart and verify added products in cart</t>
   </si>
   <si>
-    <t>Go to the product detail page to add product to cart of the same color  and size that was previously added</t>
+    <t xml:space="preserve">Add a product from the product page </t>
+  </si>
+  <si>
+    <t>The selected product is added to cart successfully</t>
+  </si>
+  <si>
+    <t>Go to the product detail page to add product to cart of the same color and size that was previously added and verify added product information in cart</t>
+  </si>
+  <si>
+    <t>Cart is empty</t>
+  </si>
+  <si>
+    <t>The information of the added products matches the one in the cart</t>
   </si>
 </sst>
 </file>
@@ -578,7 +581,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,12 +622,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -642,7 +645,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -650,16 +653,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>8</v>
@@ -668,24 +671,24 @@
         <v>9</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>8</v>
@@ -702,16 +705,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
@@ -720,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="69" x14ac:dyDescent="0.25">
@@ -728,16 +731,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>8</v>
@@ -746,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed Lesson 26 JMeter
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
@@ -581,7 +581,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="69" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
define scenario for COOLMATE-005
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-004.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncbao\Downloads\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaoNguyen\OneDrive\Máy tính\Draft Repo On Github\Draft\Katalon Projects\Test Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAD86CB-5F71-4A6B-AC91-B3AF6D52C47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COOLMATE-004" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -107,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,26 +588,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" customWidth="1"/>
+    <col min="3" max="3" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -648,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -674,7 +685,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="87" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -700,7 +711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -726,7 +737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>5</v>
       </c>

</xml_diff>